<commit_message>
Updated Jodie's tagging with missing columns
</commit_message>
<xml_diff>
--- a/Docs/Tagging/Tagging for Real - Jodie.xlsx
+++ b/Docs/Tagging/Tagging for Real - Jodie.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="81">
   <si>
     <t>artefact</t>
   </si>
@@ -241,6 +241,24 @@
   </si>
   <si>
     <t>photo</t>
+  </si>
+  <si>
+    <t>interaction</t>
+  </si>
+  <si>
+    <t>digital display</t>
+  </si>
+  <si>
+    <t>touch screen</t>
+  </si>
+  <si>
+    <t>graspables</t>
+  </si>
+  <si>
+    <t>magnifying glass</t>
+  </si>
+  <si>
+    <t>trackball</t>
   </si>
 </sst>
 </file>
@@ -347,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -371,6 +389,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -677,7 +704,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO50"/>
+  <dimension ref="A1:BT50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
@@ -688,7 +715,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>10</v>
       </c>
@@ -723,40 +750,42 @@
       <c r="AA1" s="8"/>
       <c r="AB1" s="8"/>
       <c r="AC1" s="8"/>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
       <c r="AJ1" s="8"/>
       <c r="AK1" s="8"/>
-      <c r="AL1" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="AL1" s="8"/>
       <c r="AM1" s="8"/>
       <c r="AN1" s="8"/>
       <c r="AO1" s="8"/>
       <c r="AP1" s="8"/>
       <c r="AQ1" s="8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="AR1" s="8"/>
       <c r="AS1" s="8"/>
       <c r="AT1" s="8"/>
       <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
+      <c r="AV1" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="AW1" s="8"/>
-      <c r="AX1" s="8" t="s">
-        <v>70</v>
-      </c>
+      <c r="AX1" s="8"/>
       <c r="AY1" s="8"/>
       <c r="AZ1" s="8"/>
       <c r="BA1" s="8"/>
       <c r="BB1" s="8"/>
-      <c r="BC1" s="8"/>
+      <c r="BC1" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="BD1" s="8"/>
       <c r="BE1" s="8"/>
       <c r="BF1" s="8"/>
@@ -767,12 +796,17 @@
       <c r="BK1" s="8"/>
       <c r="BL1" s="8"/>
       <c r="BM1" s="8"/>
-      <c r="BN1" s="8" t="s">
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="BO1" s="8"/>
+      <c r="BT1" s="8"/>
     </row>
-    <row r="2" spans="1:67" s="1" customFormat="1" ht="138.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:72" s="1" customFormat="1" ht="138.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -857,122 +891,137 @@
       <c r="AC2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AD2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="BA2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW2" s="2" t="s">
+      <c r="BB2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BA2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BH2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BI2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BG2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="BH2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BM2" s="2" t="s">
+      <c r="BR2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="BN2" s="3" t="s">
+      <c r="BS2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BO2" s="2" t="s">
+      <c r="BT2" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16</v>
       </c>
@@ -1011,19 +1060,19 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
-      <c r="AE3" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE3" s="5"/>
       <c r="AF3" s="5"/>
       <c r="AG3" s="5"/>
-      <c r="AH3" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
+      <c r="AJ3" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AK3" s="5"/>
       <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
+      <c r="AM3" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN3" s="5"/>
       <c r="AO3" s="5"/>
       <c r="AP3" s="5"/>
@@ -1037,14 +1086,14 @@
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
       <c r="AZ3" s="5"/>
-      <c r="BA3" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA3" s="5"/>
       <c r="BB3" s="5"/>
       <c r="BC3" s="5"/>
       <c r="BD3" s="5"/>
       <c r="BE3" s="5"/>
-      <c r="BF3" s="5"/>
+      <c r="BF3" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG3" s="5"/>
       <c r="BH3" s="5"/>
       <c r="BI3" s="5"/>
@@ -1054,8 +1103,13 @@
       <c r="BM3" s="5"/>
       <c r="BN3" s="5"/>
       <c r="BO3" s="5"/>
+      <c r="BP3" s="5"/>
+      <c r="BQ3" s="5"/>
+      <c r="BR3" s="5"/>
+      <c r="BS3" s="5"/>
+      <c r="BT3" s="5"/>
     </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>17</v>
       </c>
@@ -1103,18 +1157,18 @@
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
       <c r="AK4" s="5"/>
-      <c r="AL4" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AL4" s="5"/>
       <c r="AM4" s="5"/>
-      <c r="AN4" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AN4" s="5"/>
       <c r="AO4" s="5"/>
       <c r="AP4" s="5"/>
-      <c r="AQ4" s="5"/>
+      <c r="AQ4" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AR4" s="5"/>
-      <c r="AS4" s="5"/>
+      <c r="AS4" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AT4" s="5"/>
       <c r="AU4" s="5"/>
       <c r="AV4" s="5"/>
@@ -1137,8 +1191,13 @@
       <c r="BM4" s="5"/>
       <c r="BN4" s="5"/>
       <c r="BO4" s="5"/>
+      <c r="BP4" s="5"/>
+      <c r="BQ4" s="5"/>
+      <c r="BR4" s="5"/>
+      <c r="BS4" s="5"/>
+      <c r="BT4" s="5"/>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18</v>
       </c>
@@ -1200,17 +1259,17 @@
       <c r="AY5" s="5"/>
       <c r="AZ5" s="5"/>
       <c r="BA5" s="5"/>
-      <c r="BB5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BC5" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BB5" s="5"/>
+      <c r="BC5" s="5"/>
       <c r="BD5" s="5"/>
       <c r="BE5" s="5"/>
       <c r="BF5" s="5"/>
-      <c r="BG5" s="5"/>
-      <c r="BH5" s="5"/>
+      <c r="BG5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH5" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BI5" s="5"/>
       <c r="BJ5" s="5"/>
       <c r="BK5" s="5"/>
@@ -1218,8 +1277,13 @@
       <c r="BM5" s="5"/>
       <c r="BN5" s="5"/>
       <c r="BO5" s="5"/>
+      <c r="BP5" s="5"/>
+      <c r="BQ5" s="5"/>
+      <c r="BR5" s="5"/>
+      <c r="BS5" s="5"/>
+      <c r="BT5" s="5"/>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>19</v>
       </c>
@@ -1277,17 +1341,17 @@
       <c r="AY6" s="5"/>
       <c r="AZ6" s="5"/>
       <c r="BA6" s="5"/>
-      <c r="BB6" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BC6" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BB6" s="5"/>
+      <c r="BC6" s="5"/>
       <c r="BD6" s="5"/>
       <c r="BE6" s="5"/>
       <c r="BF6" s="5"/>
-      <c r="BG6" s="5"/>
-      <c r="BH6" s="5"/>
+      <c r="BG6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH6" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BI6" s="5"/>
       <c r="BJ6" s="5"/>
       <c r="BK6" s="5"/>
@@ -1295,8 +1359,13 @@
       <c r="BM6" s="5"/>
       <c r="BN6" s="5"/>
       <c r="BO6" s="5"/>
+      <c r="BP6" s="5"/>
+      <c r="BQ6" s="5"/>
+      <c r="BR6" s="5"/>
+      <c r="BS6" s="5"/>
+      <c r="BT6" s="5"/>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20</v>
       </c>
@@ -1369,23 +1438,28 @@
       <c r="BF7" s="5"/>
       <c r="BG7" s="5"/>
       <c r="BH7" s="5"/>
-      <c r="BI7" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI7" s="5"/>
       <c r="BJ7" s="5"/>
-      <c r="BK7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN7" s="5"/>
+      <c r="BK7" s="5"/>
+      <c r="BL7" s="5"/>
+      <c r="BM7" s="5"/>
+      <c r="BN7" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BO7" s="5"/>
+      <c r="BP7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS7" s="5"/>
+      <c r="BT7" s="5"/>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>21</v>
       </c>
@@ -1429,43 +1503,43 @@
       <c r="AE8" s="5"/>
       <c r="AF8" s="5"/>
       <c r="AG8" s="5"/>
-      <c r="AH8" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH8" s="5"/>
       <c r="AI8" s="5"/>
       <c r="AJ8" s="5"/>
       <c r="AK8" s="5"/>
-      <c r="AL8" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AL8" s="5"/>
       <c r="AM8" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AN8" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AN8" s="5"/>
       <c r="AO8" s="5"/>
       <c r="AP8" s="5"/>
-      <c r="AQ8" s="5"/>
-      <c r="AR8" s="5"/>
-      <c r="AS8" s="5"/>
-      <c r="AT8" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AQ8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS8" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT8" s="5"/>
       <c r="AU8" s="5"/>
       <c r="AV8" s="5"/>
       <c r="AW8" s="5"/>
       <c r="AX8" s="5"/>
-      <c r="AY8" s="5"/>
+      <c r="AY8" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ8" s="5"/>
-      <c r="BA8" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA8" s="5"/>
       <c r="BB8" s="5"/>
       <c r="BC8" s="5"/>
       <c r="BD8" s="5"/>
       <c r="BE8" s="5"/>
-      <c r="BF8" s="5"/>
+      <c r="BF8" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG8" s="5"/>
       <c r="BH8" s="5"/>
       <c r="BI8" s="5"/>
@@ -1475,8 +1549,13 @@
       <c r="BM8" s="5"/>
       <c r="BN8" s="5"/>
       <c r="BO8" s="5"/>
+      <c r="BP8" s="5"/>
+      <c r="BQ8" s="5"/>
+      <c r="BR8" s="5"/>
+      <c r="BS8" s="5"/>
+      <c r="BT8" s="5"/>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22</v>
       </c>
@@ -1519,19 +1598,19 @@
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
-      <c r="AE9" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE9" s="5"/>
       <c r="AF9" s="5"/>
       <c r="AG9" s="5"/>
-      <c r="AH9" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH9" s="5"/>
       <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
+      <c r="AJ9" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AK9" s="5"/>
       <c r="AL9" s="5"/>
-      <c r="AM9" s="5"/>
+      <c r="AM9" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN9" s="5"/>
       <c r="AO9" s="5"/>
       <c r="AP9" s="5"/>
@@ -1560,8 +1639,13 @@
       <c r="BM9" s="5"/>
       <c r="BN9" s="5"/>
       <c r="BO9" s="5"/>
+      <c r="BP9" s="5"/>
+      <c r="BQ9" s="5"/>
+      <c r="BR9" s="5"/>
+      <c r="BS9" s="5"/>
+      <c r="BT9" s="5"/>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>23</v>
       </c>
@@ -1606,17 +1690,17 @@
       <c r="AD10" s="5"/>
       <c r="AE10" s="5"/>
       <c r="AF10" s="5"/>
-      <c r="AG10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH10" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AG10" s="5"/>
+      <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
       <c r="AJ10" s="5"/>
       <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
+      <c r="AL10" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN10" s="5"/>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
@@ -1645,8 +1729,13 @@
       <c r="BM10" s="5"/>
       <c r="BN10" s="5"/>
       <c r="BO10" s="5"/>
+      <c r="BP10" s="5"/>
+      <c r="BQ10" s="5"/>
+      <c r="BR10" s="5"/>
+      <c r="BS10" s="5"/>
+      <c r="BT10" s="5"/>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>24</v>
       </c>
@@ -1684,44 +1773,42 @@
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
-      <c r="AD11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD11" s="5"/>
       <c r="AE11" s="5"/>
       <c r="AF11" s="5"/>
       <c r="AG11" s="5"/>
-      <c r="AH11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH11" s="5"/>
       <c r="AI11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AJ11" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AK11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ11" s="5"/>
+      <c r="AK11" s="5"/>
       <c r="AL11" s="5"/>
-      <c r="AM11" s="5"/>
-      <c r="AN11" s="5"/>
-      <c r="AO11" s="5"/>
-      <c r="AP11" s="5"/>
+      <c r="AM11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP11" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AQ11" s="5"/>
       <c r="AR11" s="5"/>
       <c r="AS11" s="5"/>
-      <c r="AT11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT11" s="5"/>
       <c r="AU11" s="5"/>
       <c r="AV11" s="5"/>
       <c r="AW11" s="5"/>
       <c r="AX11" s="5"/>
-      <c r="AY11" s="5"/>
+      <c r="AY11" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ11" s="5"/>
-      <c r="BA11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA11" s="5"/>
       <c r="BB11" s="5"/>
       <c r="BC11" s="5"/>
       <c r="BD11" s="5"/>
@@ -1733,15 +1820,22 @@
       <c r="BH11" s="5"/>
       <c r="BI11" s="5"/>
       <c r="BJ11" s="5"/>
-      <c r="BK11" s="5"/>
-      <c r="BL11" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL11" s="5"/>
       <c r="BM11" s="5"/>
       <c r="BN11" s="5"/>
       <c r="BO11" s="5"/>
+      <c r="BP11" s="5"/>
+      <c r="BQ11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR11" s="5"/>
+      <c r="BS11" s="5"/>
+      <c r="BT11" s="5"/>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1782,33 +1876,33 @@
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
-      <c r="AE12" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE12" s="5"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
-      <c r="AH12" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH12" s="5"/>
       <c r="AI12" s="5"/>
-      <c r="AJ12" s="5"/>
+      <c r="AJ12" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AK12" s="5"/>
       <c r="AL12" s="5"/>
-      <c r="AM12" s="5"/>
+      <c r="AM12" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN12" s="5"/>
       <c r="AO12" s="5"/>
       <c r="AP12" s="5"/>
       <c r="AQ12" s="5"/>
       <c r="AR12" s="5"/>
       <c r="AS12" s="5"/>
-      <c r="AT12" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT12" s="5"/>
       <c r="AU12" s="5"/>
       <c r="AV12" s="5"/>
       <c r="AW12" s="5"/>
       <c r="AX12" s="5"/>
-      <c r="AY12" s="5"/>
+      <c r="AY12" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ12" s="5"/>
       <c r="BA12" s="5"/>
       <c r="BB12" s="5"/>
@@ -1825,8 +1919,13 @@
       <c r="BM12" s="5"/>
       <c r="BN12" s="5"/>
       <c r="BO12" s="5"/>
+      <c r="BP12" s="5"/>
+      <c r="BQ12" s="5"/>
+      <c r="BR12" s="5"/>
+      <c r="BS12" s="5"/>
+      <c r="BT12" s="5"/>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
@@ -1869,45 +1968,50 @@
       <c r="AJ13" s="5"/>
       <c r="AK13" s="5"/>
       <c r="AL13" s="5"/>
-      <c r="AM13" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM13" s="5"/>
       <c r="AN13" s="5"/>
       <c r="AO13" s="5"/>
       <c r="AP13" s="5"/>
       <c r="AQ13" s="5"/>
-      <c r="AR13" s="5"/>
+      <c r="AR13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AS13" s="5"/>
-      <c r="AT13" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT13" s="5"/>
       <c r="AU13" s="5"/>
       <c r="AV13" s="5"/>
       <c r="AW13" s="5"/>
       <c r="AX13" s="5"/>
-      <c r="AY13" s="5"/>
+      <c r="AY13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ13" s="5"/>
-      <c r="BA13" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA13" s="5"/>
       <c r="BB13" s="5"/>
       <c r="BC13" s="5"/>
       <c r="BD13" s="5"/>
       <c r="BE13" s="5"/>
-      <c r="BF13" s="5"/>
+      <c r="BF13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG13" s="5"/>
-      <c r="BH13" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BH13" s="5"/>
       <c r="BI13" s="5"/>
       <c r="BJ13" s="5"/>
       <c r="BK13" s="5"/>
       <c r="BL13" s="5"/>
-      <c r="BM13" s="5"/>
+      <c r="BM13" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BN13" s="5"/>
       <c r="BO13" s="5"/>
+      <c r="BP13" s="5"/>
+      <c r="BQ13" s="5"/>
+      <c r="BR13" s="5"/>
+      <c r="BS13" s="5"/>
+      <c r="BT13" s="5"/>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>27</v>
       </c>
@@ -1945,54 +2049,59 @@
       <c r="AE14" s="5"/>
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
-      <c r="AH14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI14" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AJ14" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH14" s="5"/>
+      <c r="AI14" s="5"/>
+      <c r="AJ14" s="5"/>
       <c r="AK14" s="5"/>
       <c r="AL14" s="5"/>
-      <c r="AM14" s="5"/>
-      <c r="AN14" s="5"/>
-      <c r="AO14" s="5"/>
+      <c r="AM14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO14" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AP14" s="5"/>
       <c r="AQ14" s="5"/>
       <c r="AR14" s="5"/>
       <c r="AS14" s="5"/>
-      <c r="AT14" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT14" s="5"/>
       <c r="AU14" s="5"/>
       <c r="AV14" s="5"/>
       <c r="AW14" s="5"/>
       <c r="AX14" s="5"/>
-      <c r="AY14" s="5"/>
+      <c r="AY14" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ14" s="5"/>
       <c r="BA14" s="5"/>
       <c r="BB14" s="5"/>
       <c r="BC14" s="5"/>
       <c r="BD14" s="5"/>
       <c r="BE14" s="5"/>
-      <c r="BF14" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF14" s="5"/>
       <c r="BG14" s="5"/>
       <c r="BH14" s="5"/>
       <c r="BI14" s="5"/>
       <c r="BJ14" s="5"/>
-      <c r="BK14" s="5"/>
-      <c r="BL14" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL14" s="5"/>
       <c r="BM14" s="5"/>
       <c r="BN14" s="5"/>
       <c r="BO14" s="5"/>
+      <c r="BP14" s="5"/>
+      <c r="BQ14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR14" s="5"/>
+      <c r="BS14" s="5"/>
+      <c r="BT14" s="5"/>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>28</v>
       </c>
@@ -2041,24 +2150,24 @@
       <c r="AP15" s="5"/>
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
-      <c r="AS15" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AS15" s="5"/>
       <c r="AT15" s="5"/>
       <c r="AU15" s="5"/>
       <c r="AV15" s="5"/>
       <c r="AW15" s="5"/>
-      <c r="AX15" s="5"/>
+      <c r="AX15" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AY15" s="5"/>
       <c r="AZ15" s="5"/>
-      <c r="BA15" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA15" s="5"/>
       <c r="BB15" s="5"/>
       <c r="BC15" s="5"/>
       <c r="BD15" s="5"/>
       <c r="BE15" s="5"/>
-      <c r="BF15" s="5"/>
+      <c r="BF15" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG15" s="5"/>
       <c r="BH15" s="5"/>
       <c r="BI15" s="5"/>
@@ -2067,11 +2176,16 @@
       <c r="BL15" s="5"/>
       <c r="BM15" s="5"/>
       <c r="BN15" s="5"/>
-      <c r="BO15" s="5" t="s">
+      <c r="BO15" s="5"/>
+      <c r="BP15" s="5"/>
+      <c r="BQ15" s="5"/>
+      <c r="BR15" s="5"/>
+      <c r="BS15" s="5"/>
+      <c r="BT15" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>29</v>
       </c>
@@ -2111,9 +2225,7 @@
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
-      <c r="AD16" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD16" s="5"/>
       <c r="AE16" s="5"/>
       <c r="AF16" s="5"/>
       <c r="AG16" s="5"/>
@@ -2139,19 +2251,19 @@
       <c r="AU16" s="5"/>
       <c r="AV16" s="5"/>
       <c r="AW16" s="5"/>
-      <c r="AX16" s="5"/>
+      <c r="AX16" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AY16" s="5"/>
       <c r="AZ16" s="5"/>
-      <c r="BA16" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA16" s="5"/>
       <c r="BB16" s="5"/>
       <c r="BC16" s="5"/>
       <c r="BD16" s="5"/>
-      <c r="BE16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF16" s="5"/>
+      <c r="BE16" s="5"/>
+      <c r="BF16" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG16" s="5"/>
       <c r="BH16" s="5"/>
       <c r="BI16" s="5"/>
@@ -2159,18 +2271,25 @@
         <v>71</v>
       </c>
       <c r="BK16" s="5"/>
-      <c r="BL16" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL16" s="5"/>
       <c r="BM16" s="5"/>
-      <c r="BN16" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BN16" s="5"/>
       <c r="BO16" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="BP16" s="5"/>
+      <c r="BQ16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR16" s="5"/>
+      <c r="BS16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT16" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>30</v>
       </c>
@@ -2212,9 +2331,7 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
-      <c r="AD17" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD17" s="5"/>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="5"/>
@@ -2233,26 +2350,26 @@
       <c r="AP17" s="5"/>
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
-      <c r="AS17" s="5"/>
+      <c r="AS17" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AT17" s="5"/>
-      <c r="AU17" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AU17" s="5"/>
       <c r="AV17" s="5"/>
       <c r="AW17" s="5"/>
       <c r="AX17" s="5"/>
       <c r="AY17" s="5"/>
-      <c r="AZ17" s="5"/>
-      <c r="BA17" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AZ17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA17" s="5"/>
       <c r="BB17" s="5"/>
       <c r="BC17" s="5"/>
       <c r="BD17" s="5"/>
-      <c r="BE17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF17" s="5"/>
+      <c r="BE17" s="5"/>
+      <c r="BF17" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG17" s="5"/>
       <c r="BH17" s="5"/>
       <c r="BI17" s="5"/>
@@ -2260,16 +2377,23 @@
         <v>71</v>
       </c>
       <c r="BK17" s="5"/>
-      <c r="BL17" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL17" s="5"/>
       <c r="BM17" s="5"/>
-      <c r="BN17" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BO17" s="5"/>
+      <c r="BN17" s="5"/>
+      <c r="BO17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BP17" s="5"/>
+      <c r="BQ17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR17" s="5"/>
+      <c r="BS17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT17" s="5"/>
     </row>
-    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>31</v>
       </c>
@@ -2317,9 +2441,7 @@
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
-      <c r="AD18" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD18" s="5"/>
       <c r="AE18" s="5"/>
       <c r="AF18" s="5"/>
       <c r="AG18" s="5"/>
@@ -2327,60 +2449,67 @@
       <c r="AI18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AJ18" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ18" s="5"/>
       <c r="AK18" s="5"/>
-      <c r="AL18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AM18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN18" s="5"/>
-      <c r="AO18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO18" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AP18" s="5"/>
       <c r="AQ18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AR18" s="5"/>
+      <c r="AR18" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AS18" s="5"/>
-      <c r="AT18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AV18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AW18" s="5"/>
       <c r="AX18" s="5"/>
       <c r="AY18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AZ18" s="5"/>
-      <c r="BA18" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AZ18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA18" s="5"/>
       <c r="BB18" s="5"/>
       <c r="BC18" s="5"/>
-      <c r="BD18" s="5"/>
-      <c r="BE18" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF18" s="5"/>
+      <c r="BD18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BE18" s="5"/>
+      <c r="BF18" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG18" s="5"/>
       <c r="BH18" s="5"/>
       <c r="BI18" s="5"/>
-      <c r="BJ18" s="5"/>
+      <c r="BJ18" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BK18" s="5"/>
-      <c r="BL18" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL18" s="5"/>
       <c r="BM18" s="5"/>
       <c r="BN18" s="5"/>
       <c r="BO18" s="5"/>
+      <c r="BP18" s="5"/>
+      <c r="BQ18" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR18" s="5"/>
+      <c r="BS18" s="5"/>
+      <c r="BT18" s="5"/>
     </row>
-    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>32</v>
       </c>
@@ -2450,8 +2579,13 @@
       <c r="BM19" s="6"/>
       <c r="BN19" s="6"/>
       <c r="BO19" s="6"/>
+      <c r="BP19" s="6"/>
+      <c r="BQ19" s="6"/>
+      <c r="BR19" s="6"/>
+      <c r="BS19" s="6"/>
+      <c r="BT19" s="6"/>
     </row>
-    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>33</v>
       </c>
@@ -2487,9 +2621,7 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
-      <c r="AD20" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD20" s="5"/>
       <c r="AE20" s="5"/>
       <c r="AF20" s="5"/>
       <c r="AG20" s="5"/>
@@ -2500,22 +2632,22 @@
       <c r="AJ20" s="5"/>
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
-      <c r="AM20" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM20" s="5"/>
       <c r="AN20" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO20" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP20" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
       <c r="AQ20" s="5"/>
-      <c r="AR20" s="5"/>
-      <c r="AS20" s="5"/>
-      <c r="AT20" s="5"/>
+      <c r="AR20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT20" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AU20" s="5" t="s">
         <v>71</v>
       </c>
@@ -2523,14 +2655,14 @@
       <c r="AW20" s="5"/>
       <c r="AX20" s="5"/>
       <c r="AY20" s="5"/>
-      <c r="AZ20" s="5"/>
+      <c r="AZ20" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BA20" s="5"/>
       <c r="BB20" s="5"/>
       <c r="BC20" s="5"/>
       <c r="BD20" s="5"/>
-      <c r="BE20" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BE20" s="5"/>
       <c r="BF20" s="5"/>
       <c r="BG20" s="5"/>
       <c r="BH20" s="5"/>
@@ -2545,8 +2677,15 @@
       <c r="BO20" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="BP20" s="5"/>
+      <c r="BQ20" s="5"/>
+      <c r="BR20" s="5"/>
+      <c r="BS20" s="5"/>
+      <c r="BT20" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>34</v>
       </c>
@@ -2605,14 +2744,14 @@
       <c r="AX21" s="5"/>
       <c r="AY21" s="5"/>
       <c r="AZ21" s="5"/>
-      <c r="BA21" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA21" s="5"/>
       <c r="BB21" s="5"/>
       <c r="BC21" s="5"/>
       <c r="BD21" s="5"/>
       <c r="BE21" s="5"/>
-      <c r="BF21" s="5"/>
+      <c r="BF21" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG21" s="5"/>
       <c r="BH21" s="5"/>
       <c r="BI21" s="5"/>
@@ -2622,8 +2761,13 @@
       <c r="BM21" s="5"/>
       <c r="BN21" s="5"/>
       <c r="BO21" s="5"/>
+      <c r="BP21" s="5"/>
+      <c r="BQ21" s="5"/>
+      <c r="BR21" s="5"/>
+      <c r="BS21" s="5"/>
+      <c r="BT21" s="5"/>
     </row>
-    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>35</v>
       </c>
@@ -2667,15 +2811,11 @@
       <c r="AA22" s="5"/>
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
-      <c r="AD22" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD22" s="5"/>
       <c r="AE22" s="5"/>
       <c r="AF22" s="5"/>
       <c r="AG22" s="5"/>
-      <c r="AH22" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH22" s="5"/>
       <c r="AI22" s="5" t="s">
         <v>71</v>
       </c>
@@ -2688,55 +2828,64 @@
       <c r="AN22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR22" s="5"/>
-      <c r="AS22" s="5"/>
-      <c r="AT22" s="5"/>
+      <c r="AO22" s="5"/>
+      <c r="AP22" s="5"/>
+      <c r="AQ22" s="5"/>
+      <c r="AR22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT22" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AU22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AV22" s="5"/>
+      <c r="AV22" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AW22" s="5"/>
-      <c r="AX22" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AX22" s="5"/>
       <c r="AY22" s="5"/>
-      <c r="AZ22" s="5"/>
-      <c r="BA22" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AZ22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA22" s="5"/>
       <c r="BB22" s="5"/>
-      <c r="BC22" s="5"/>
+      <c r="BC22" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BD22" s="5"/>
-      <c r="BE22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BF22" s="5"/>
+      <c r="BE22" s="5"/>
+      <c r="BF22" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG22" s="5"/>
       <c r="BH22" s="5"/>
       <c r="BI22" s="5"/>
-      <c r="BJ22" s="5"/>
+      <c r="BJ22" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BK22" s="5"/>
-      <c r="BL22" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM22" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL22" s="5"/>
+      <c r="BM22" s="5"/>
       <c r="BN22" s="5"/>
-      <c r="BO22" s="5" t="s">
+      <c r="BO22" s="5"/>
+      <c r="BP22" s="5"/>
+      <c r="BQ22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS22" s="5"/>
+      <c r="BT22" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>36</v>
       </c>
@@ -2776,68 +2925,75 @@
       <c r="AA23" s="5"/>
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
-      <c r="AD23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD23" s="5"/>
       <c r="AE23" s="5"/>
-      <c r="AF23" s="5"/>
+      <c r="AF23" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AG23" s="5"/>
-      <c r="AH23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH23" s="5"/>
       <c r="AI23" s="5" t="s">
         <v>71</v>
       </c>
       <c r="AJ23" s="5"/>
       <c r="AK23" s="5"/>
       <c r="AL23" s="5"/>
-      <c r="AM23" s="5"/>
+      <c r="AM23" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO23" s="5"/>
       <c r="AP23" s="5"/>
       <c r="AQ23" s="5"/>
       <c r="AR23" s="5"/>
-      <c r="AS23" s="5"/>
+      <c r="AS23" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AT23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AU23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AU23" s="5"/>
       <c r="AV23" s="5"/>
       <c r="AW23" s="5"/>
       <c r="AX23" s="5"/>
-      <c r="AY23" s="5"/>
-      <c r="AZ23" s="5"/>
-      <c r="BA23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AY23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BA23" s="5"/>
       <c r="BB23" s="5"/>
       <c r="BC23" s="5"/>
       <c r="BD23" s="5"/>
       <c r="BE23" s="5"/>
-      <c r="BF23" s="5"/>
+      <c r="BF23" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG23" s="5"/>
       <c r="BH23" s="5"/>
-      <c r="BI23" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BJ23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI23" s="5"/>
+      <c r="BJ23" s="5"/>
       <c r="BK23" s="5"/>
-      <c r="BL23" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL23" s="5"/>
       <c r="BM23" s="5"/>
-      <c r="BN23" s="5"/>
-      <c r="BO23" s="5"/>
+      <c r="BN23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BP23" s="5"/>
+      <c r="BQ23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR23" s="5"/>
+      <c r="BS23" s="5"/>
+      <c r="BT23" s="5"/>
     </row>
-    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>37</v>
       </c>
@@ -2885,9 +3041,7 @@
       <c r="AC24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AD24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD24" s="7"/>
       <c r="AE24" s="7"/>
       <c r="AF24" s="7"/>
       <c r="AG24" s="7"/>
@@ -2895,29 +3049,29 @@
       <c r="AI24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AJ24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ24" s="7"/>
       <c r="AK24" s="7"/>
       <c r="AL24" s="7"/>
       <c r="AM24" s="7"/>
       <c r="AN24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AO24" s="7"/>
+      <c r="AO24" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AP24" s="7"/>
       <c r="AQ24" s="7"/>
       <c r="AR24" s="7"/>
       <c r="AS24" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AT24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT24" s="7"/>
       <c r="AU24" s="7"/>
       <c r="AV24" s="7"/>
       <c r="AW24" s="7"/>
-      <c r="AX24" s="7"/>
+      <c r="AX24" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AY24" s="7" t="s">
         <v>71</v>
       </c>
@@ -2925,30 +3079,37 @@
       <c r="BA24" s="7"/>
       <c r="BB24" s="7"/>
       <c r="BC24" s="7"/>
-      <c r="BD24" s="7"/>
+      <c r="BD24" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="BE24" s="7"/>
       <c r="BF24" s="7"/>
       <c r="BG24" s="7"/>
       <c r="BH24" s="7"/>
-      <c r="BI24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BJ24" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI24" s="7"/>
+      <c r="BJ24" s="7"/>
       <c r="BK24" s="7"/>
-      <c r="BL24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN24" s="7"/>
+      <c r="BL24" s="7"/>
+      <c r="BM24" s="7"/>
+      <c r="BN24" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="BO24" s="7" t="s">
         <v>71</v>
       </c>
+      <c r="BP24" s="7"/>
+      <c r="BQ24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS24" s="7"/>
+      <c r="BT24" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>38</v>
       </c>
@@ -2994,12 +3155,14 @@
       <c r="AC25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AD25" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD25" s="7"/>
       <c r="AE25" s="7"/>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="7"/>
+      <c r="AF25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG25" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AH25" s="7"/>
       <c r="AI25" s="7" t="s">
         <v>71</v>
@@ -3011,9 +3174,7 @@
       <c r="AN25" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AO25" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO25" s="7"/>
       <c r="AP25" s="7"/>
       <c r="AQ25" s="7"/>
       <c r="AR25" s="7"/>
@@ -3026,7 +3187,9 @@
       <c r="AU25" s="7"/>
       <c r="AV25" s="7"/>
       <c r="AW25" s="7"/>
-      <c r="AX25" s="7"/>
+      <c r="AX25" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AY25" s="7" t="s">
         <v>71</v>
       </c>
@@ -3034,30 +3197,37 @@
       <c r="BA25" s="7"/>
       <c r="BB25" s="7"/>
       <c r="BC25" s="7"/>
-      <c r="BD25" s="7"/>
+      <c r="BD25" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="BE25" s="7"/>
-      <c r="BF25" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF25" s="7"/>
       <c r="BG25" s="7"/>
       <c r="BH25" s="7"/>
       <c r="BI25" s="7"/>
-      <c r="BJ25" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK25" s="7"/>
-      <c r="BL25" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BJ25" s="7"/>
+      <c r="BK25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL25" s="7"/>
       <c r="BM25" s="7"/>
-      <c r="BN25" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BN25" s="7"/>
       <c r="BO25" s="7" t="s">
         <v>71</v>
       </c>
+      <c r="BP25" s="7"/>
+      <c r="BQ25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR25" s="7"/>
+      <c r="BS25" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT25" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>39</v>
       </c>
@@ -3099,54 +3269,59 @@
       <c r="AE26" s="5"/>
       <c r="AF26" s="5"/>
       <c r="AG26" s="5"/>
-      <c r="AH26" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH26" s="5"/>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
       <c r="AK26" s="5"/>
       <c r="AL26" s="5"/>
-      <c r="AM26" s="5"/>
-      <c r="AN26" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN26" s="5"/>
       <c r="AO26" s="5"/>
-      <c r="AP26" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AP26" s="5"/>
       <c r="AQ26" s="5"/>
       <c r="AR26" s="5"/>
-      <c r="AS26" s="5"/>
-      <c r="AT26" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AU26" s="5"/>
+      <c r="AS26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT26" s="5"/>
+      <c r="AU26" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AV26" s="5"/>
       <c r="AW26" s="5"/>
       <c r="AX26" s="5"/>
-      <c r="AY26" s="5"/>
+      <c r="AY26" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ26" s="5"/>
       <c r="BA26" s="5"/>
       <c r="BB26" s="5"/>
       <c r="BC26" s="5"/>
       <c r="BD26" s="5"/>
       <c r="BE26" s="5"/>
-      <c r="BF26" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF26" s="5"/>
       <c r="BG26" s="5"/>
       <c r="BH26" s="5"/>
       <c r="BI26" s="5"/>
       <c r="BJ26" s="5"/>
-      <c r="BK26" s="5"/>
-      <c r="BL26" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL26" s="5"/>
       <c r="BM26" s="5"/>
       <c r="BN26" s="5"/>
       <c r="BO26" s="5"/>
+      <c r="BP26" s="5"/>
+      <c r="BQ26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR26" s="5"/>
+      <c r="BS26" s="5"/>
+      <c r="BT26" s="5"/>
     </row>
-    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>40</v>
       </c>
@@ -3186,30 +3361,24 @@
       <c r="AA27" s="5"/>
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
-      <c r="AD27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD27" s="5"/>
       <c r="AE27" s="5"/>
       <c r="AF27" s="5"/>
       <c r="AG27" s="5"/>
-      <c r="AH27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH27" s="5"/>
       <c r="AI27" s="5" t="s">
         <v>71</v>
       </c>
       <c r="AJ27" s="5"/>
-      <c r="AK27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AK27" s="5"/>
       <c r="AL27" s="5"/>
-      <c r="AM27" s="5"/>
+      <c r="AM27" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO27" s="5"/>
       <c r="AP27" s="5" t="s">
         <v>71</v>
       </c>
@@ -3221,15 +3390,19 @@
       <c r="AT27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AU27" s="5"/>
+      <c r="AU27" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AV27" s="5"/>
       <c r="AW27" s="5"/>
-      <c r="AX27" s="5"/>
-      <c r="AY27" s="5"/>
+      <c r="AX27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY27" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ27" s="5"/>
-      <c r="BA27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA27" s="5"/>
       <c r="BB27" s="5"/>
       <c r="BC27" s="5"/>
       <c r="BD27" s="5"/>
@@ -3240,24 +3413,31 @@
       <c r="BG27" s="5"/>
       <c r="BH27" s="5"/>
       <c r="BI27" s="5"/>
-      <c r="BJ27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK27" s="5"/>
-      <c r="BL27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM27" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN27" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BJ27" s="5"/>
+      <c r="BK27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL27" s="5"/>
+      <c r="BM27" s="5"/>
+      <c r="BN27" s="5"/>
       <c r="BO27" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="BP27" s="5"/>
+      <c r="BQ27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT27" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>41</v>
       </c>
@@ -3299,66 +3479,73 @@
       <c r="AA28" s="5"/>
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
-      <c r="AD28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD28" s="5"/>
       <c r="AE28" s="5"/>
       <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI28" s="5"/>
+      <c r="AG28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AJ28" s="5"/>
       <c r="AK28" s="5"/>
       <c r="AL28" s="5"/>
-      <c r="AM28" s="5"/>
-      <c r="AN28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
       <c r="AQ28" s="5"/>
       <c r="AR28" s="5"/>
-      <c r="AS28" s="5"/>
+      <c r="AS28" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AT28" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AU28" s="5"/>
-      <c r="AV28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AU28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AV28" s="5"/>
       <c r="AW28" s="5"/>
       <c r="AX28" s="5"/>
-      <c r="AY28" s="5"/>
+      <c r="AY28" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ28" s="5"/>
-      <c r="BA28" s="5"/>
+      <c r="BA28" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BB28" s="5"/>
       <c r="BC28" s="5"/>
       <c r="BD28" s="5"/>
       <c r="BE28" s="5"/>
-      <c r="BF28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF28" s="5"/>
       <c r="BG28" s="5"/>
       <c r="BH28" s="5"/>
       <c r="BI28" s="5"/>
       <c r="BJ28" s="5"/>
-      <c r="BK28" s="5"/>
-      <c r="BL28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL28" s="5"/>
       <c r="BM28" s="5"/>
-      <c r="BN28" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BN28" s="5"/>
       <c r="BO28" s="5"/>
+      <c r="BP28" s="5"/>
+      <c r="BQ28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR28" s="5"/>
+      <c r="BS28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT28" s="5"/>
     </row>
-    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>42</v>
       </c>
@@ -3428,8 +3615,13 @@
       <c r="BM29" s="6"/>
       <c r="BN29" s="6"/>
       <c r="BO29" s="6"/>
+      <c r="BP29" s="6"/>
+      <c r="BQ29" s="6"/>
+      <c r="BR29" s="6"/>
+      <c r="BS29" s="6"/>
+      <c r="BT29" s="6"/>
     </row>
-    <row r="30" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>43</v>
       </c>
@@ -3475,41 +3667,45 @@
       <c r="AC30" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AD30" s="5"/>
-      <c r="AE30" s="5"/>
+      <c r="AD30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE30" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AF30" s="5"/>
       <c r="AG30" s="5"/>
-      <c r="AH30" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH30" s="5"/>
       <c r="AI30" s="5"/>
       <c r="AJ30" s="5"/>
       <c r="AK30" s="5"/>
       <c r="AL30" s="5"/>
-      <c r="AM30" s="5"/>
+      <c r="AM30" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN30" s="5"/>
       <c r="AO30" s="5"/>
       <c r="AP30" s="5"/>
       <c r="AQ30" s="5"/>
       <c r="AR30" s="5"/>
       <c r="AS30" s="5"/>
-      <c r="AT30" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT30" s="5"/>
       <c r="AU30" s="5"/>
       <c r="AV30" s="5"/>
       <c r="AW30" s="5"/>
       <c r="AX30" s="5"/>
-      <c r="AY30" s="5"/>
+      <c r="AY30" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ30" s="5"/>
-      <c r="BA30" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA30" s="5"/>
       <c r="BB30" s="5"/>
       <c r="BC30" s="5"/>
       <c r="BD30" s="5"/>
       <c r="BE30" s="5"/>
-      <c r="BF30" s="5"/>
+      <c r="BF30" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG30" s="5"/>
       <c r="BH30" s="5"/>
       <c r="BI30" s="5"/>
@@ -3519,8 +3715,13 @@
       <c r="BM30" s="5"/>
       <c r="BN30" s="5"/>
       <c r="BO30" s="5"/>
+      <c r="BP30" s="5"/>
+      <c r="BQ30" s="5"/>
+      <c r="BR30" s="5"/>
+      <c r="BS30" s="5"/>
+      <c r="BT30" s="5"/>
     </row>
-    <row r="31" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>44</v>
       </c>
@@ -3565,9 +3766,7 @@
       <c r="AF31" s="5"/>
       <c r="AG31" s="5"/>
       <c r="AH31" s="5"/>
-      <c r="AI31" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AI31" s="5"/>
       <c r="AJ31" s="5"/>
       <c r="AK31" s="5"/>
       <c r="AL31" s="5"/>
@@ -3579,10 +3778,10 @@
       <c r="AP31" s="5"/>
       <c r="AQ31" s="5"/>
       <c r="AR31" s="5"/>
-      <c r="AS31" s="5"/>
-      <c r="AT31" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AS31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT31" s="5"/>
       <c r="AU31" s="5"/>
       <c r="AV31" s="5"/>
       <c r="AW31" s="5"/>
@@ -3594,22 +3793,29 @@
       <c r="BA31" s="5"/>
       <c r="BB31" s="5"/>
       <c r="BC31" s="5"/>
-      <c r="BD31" s="5"/>
+      <c r="BD31" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BE31" s="5"/>
       <c r="BF31" s="5"/>
       <c r="BG31" s="5"/>
       <c r="BH31" s="5"/>
-      <c r="BI31" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI31" s="5"/>
       <c r="BJ31" s="5"/>
       <c r="BK31" s="5"/>
       <c r="BL31" s="5"/>
       <c r="BM31" s="5"/>
-      <c r="BN31" s="5"/>
+      <c r="BN31" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BO31" s="5"/>
+      <c r="BP31" s="5"/>
+      <c r="BQ31" s="5"/>
+      <c r="BR31" s="5"/>
+      <c r="BS31" s="5"/>
+      <c r="BT31" s="5"/>
     </row>
-    <row r="32" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>45</v>
       </c>
@@ -3679,8 +3885,13 @@
       <c r="BM32" s="6"/>
       <c r="BN32" s="6"/>
       <c r="BO32" s="6"/>
+      <c r="BP32" s="6"/>
+      <c r="BQ32" s="6"/>
+      <c r="BR32" s="6"/>
+      <c r="BS32" s="6"/>
+      <c r="BT32" s="6"/>
     </row>
-    <row r="33" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>46</v>
       </c>
@@ -3726,28 +3937,24 @@
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
-      <c r="AD33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD33" s="5"/>
       <c r="AE33" s="5"/>
-      <c r="AF33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AF33" s="5"/>
       <c r="AG33" s="5"/>
-      <c r="AH33" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AJ33" s="5"/>
-      <c r="AK33" s="5"/>
+      <c r="AK33" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AL33" s="5"/>
-      <c r="AM33" s="5"/>
-      <c r="AN33" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AM33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN33" s="5"/>
+      <c r="AO33" s="5"/>
       <c r="AP33" s="5"/>
       <c r="AQ33" s="5"/>
       <c r="AR33" s="5"/>
@@ -3760,12 +3967,14 @@
       <c r="AU33" s="5"/>
       <c r="AV33" s="5"/>
       <c r="AW33" s="5"/>
-      <c r="AX33" s="5"/>
-      <c r="AY33" s="5"/>
+      <c r="AX33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY33" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ33" s="5"/>
-      <c r="BA33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA33" s="5"/>
       <c r="BB33" s="5"/>
       <c r="BC33" s="5"/>
       <c r="BD33" s="5"/>
@@ -3777,15 +3986,22 @@
       <c r="BH33" s="5"/>
       <c r="BI33" s="5"/>
       <c r="BJ33" s="5"/>
-      <c r="BK33" s="5"/>
-      <c r="BL33" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL33" s="5"/>
       <c r="BM33" s="5"/>
       <c r="BN33" s="5"/>
       <c r="BO33" s="5"/>
+      <c r="BP33" s="5"/>
+      <c r="BQ33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR33" s="5"/>
+      <c r="BS33" s="5"/>
+      <c r="BT33" s="5"/>
     </row>
-    <row r="34" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>47</v>
       </c>
@@ -3855,8 +4071,13 @@
       <c r="BM34" s="6"/>
       <c r="BN34" s="6"/>
       <c r="BO34" s="6"/>
+      <c r="BP34" s="6"/>
+      <c r="BQ34" s="6"/>
+      <c r="BR34" s="6"/>
+      <c r="BS34" s="6"/>
+      <c r="BT34" s="6"/>
     </row>
-    <row r="35" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>48</v>
       </c>
@@ -3926,8 +4147,13 @@
       <c r="BM35" s="6"/>
       <c r="BN35" s="6"/>
       <c r="BO35" s="6"/>
+      <c r="BP35" s="6"/>
+      <c r="BQ35" s="6"/>
+      <c r="BR35" s="6"/>
+      <c r="BS35" s="6"/>
+      <c r="BT35" s="6"/>
     </row>
-    <row r="36" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>49</v>
       </c>
@@ -3975,39 +4201,37 @@
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
       <c r="AE36" s="5"/>
-      <c r="AF36" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AF36" s="5"/>
       <c r="AG36" s="5"/>
       <c r="AH36" s="5"/>
-      <c r="AI36" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AI36" s="5"/>
       <c r="AJ36" s="5"/>
-      <c r="AK36" s="5"/>
+      <c r="AK36" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AL36" s="5"/>
       <c r="AM36" s="5"/>
-      <c r="AN36" s="5"/>
+      <c r="AN36" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AO36" s="5"/>
       <c r="AP36" s="5"/>
       <c r="AQ36" s="5"/>
       <c r="AR36" s="5"/>
       <c r="AS36" s="5"/>
-      <c r="AT36" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT36" s="5"/>
       <c r="AU36" s="5"/>
       <c r="AV36" s="5"/>
-      <c r="AW36" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AW36" s="5"/>
       <c r="AX36" s="5"/>
-      <c r="AY36" s="5"/>
+      <c r="AY36" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ36" s="5"/>
-      <c r="BA36" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BB36" s="5"/>
+      <c r="BA36" s="5"/>
+      <c r="BB36" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BC36" s="5"/>
       <c r="BD36" s="5"/>
       <c r="BE36" s="5"/>
@@ -4018,17 +4242,24 @@
       <c r="BH36" s="5"/>
       <c r="BI36" s="5"/>
       <c r="BJ36" s="5"/>
-      <c r="BK36" s="5"/>
-      <c r="BL36" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM36" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL36" s="5"/>
+      <c r="BM36" s="5"/>
       <c r="BN36" s="5"/>
       <c r="BO36" s="5"/>
+      <c r="BP36" s="5"/>
+      <c r="BQ36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS36" s="5"/>
+      <c r="BT36" s="5"/>
     </row>
-    <row r="37" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50</v>
       </c>
@@ -4076,52 +4307,57 @@
       <c r="AE37" s="5"/>
       <c r="AF37" s="5"/>
       <c r="AG37" s="5"/>
-      <c r="AH37" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH37" s="5"/>
       <c r="AI37" s="5"/>
       <c r="AJ37" s="5"/>
-      <c r="AK37" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AK37" s="5"/>
       <c r="AL37" s="5"/>
-      <c r="AM37" s="5"/>
+      <c r="AM37" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN37" s="5"/>
       <c r="AO37" s="5"/>
-      <c r="AP37" s="5"/>
+      <c r="AP37" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AQ37" s="5"/>
       <c r="AR37" s="5"/>
       <c r="AS37" s="5"/>
-      <c r="AT37" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT37" s="5"/>
       <c r="AU37" s="5"/>
       <c r="AV37" s="5"/>
       <c r="AW37" s="5"/>
       <c r="AX37" s="5"/>
-      <c r="AY37" s="5"/>
+      <c r="AY37" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ37" s="5"/>
       <c r="BA37" s="5"/>
       <c r="BB37" s="5"/>
       <c r="BC37" s="5"/>
       <c r="BD37" s="5"/>
       <c r="BE37" s="5"/>
-      <c r="BF37" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF37" s="5"/>
       <c r="BG37" s="5"/>
       <c r="BH37" s="5"/>
       <c r="BI37" s="5"/>
-      <c r="BJ37" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BK37" s="5"/>
+      <c r="BJ37" s="5"/>
+      <c r="BK37" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BL37" s="5"/>
       <c r="BM37" s="5"/>
       <c r="BN37" s="5"/>
-      <c r="BO37" s="5"/>
+      <c r="BO37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BP37" s="5"/>
+      <c r="BQ37" s="5"/>
+      <c r="BR37" s="5"/>
+      <c r="BS37" s="5"/>
+      <c r="BT37" s="5"/>
     </row>
-    <row r="38" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>51</v>
       </c>
@@ -4168,51 +4404,56 @@
       <c r="AF38" s="7"/>
       <c r="AG38" s="7"/>
       <c r="AH38" s="7"/>
-      <c r="AI38" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AI38" s="7"/>
       <c r="AJ38" s="7"/>
       <c r="AK38" s="7"/>
       <c r="AL38" s="7"/>
       <c r="AM38" s="7"/>
-      <c r="AN38" s="7"/>
+      <c r="AN38" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AO38" s="7"/>
       <c r="AP38" s="7"/>
       <c r="AQ38" s="7"/>
-      <c r="AR38" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="AR38" s="7"/>
       <c r="AS38" s="7"/>
       <c r="AT38" s="7"/>
       <c r="AU38" s="7"/>
       <c r="AV38" s="7"/>
-      <c r="AW38" s="7"/>
+      <c r="AW38" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="AX38" s="7"/>
       <c r="AY38" s="7"/>
       <c r="AZ38" s="7"/>
       <c r="BA38" s="7"/>
       <c r="BB38" s="7"/>
       <c r="BC38" s="7"/>
-      <c r="BD38" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BD38" s="7"/>
       <c r="BE38" s="7"/>
       <c r="BF38" s="7"/>
       <c r="BG38" s="7"/>
       <c r="BH38" s="7"/>
-      <c r="BI38" s="7"/>
+      <c r="BI38" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="BJ38" s="7"/>
-      <c r="BK38" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL38" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK38" s="7"/>
+      <c r="BL38" s="7"/>
       <c r="BM38" s="7"/>
       <c r="BN38" s="7"/>
       <c r="BO38" s="7"/>
+      <c r="BP38" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ38" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR38" s="7"/>
+      <c r="BS38" s="7"/>
+      <c r="BT38" s="7"/>
     </row>
-    <row r="39" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>52</v>
       </c>
@@ -4282,8 +4523,13 @@
       <c r="BM39" s="6"/>
       <c r="BN39" s="6"/>
       <c r="BO39" s="6"/>
+      <c r="BP39" s="6"/>
+      <c r="BQ39" s="6"/>
+      <c r="BR39" s="6"/>
+      <c r="BS39" s="6"/>
+      <c r="BT39" s="6"/>
     </row>
-    <row r="40" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>53</v>
       </c>
@@ -4323,22 +4569,20 @@
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
       <c r="AC40" s="5"/>
-      <c r="AD40" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD40" s="5"/>
       <c r="AE40" s="5"/>
       <c r="AF40" s="5"/>
       <c r="AG40" s="5"/>
-      <c r="AH40" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH40" s="5"/>
       <c r="AI40" s="5" t="s">
         <v>71</v>
       </c>
       <c r="AJ40" s="5"/>
       <c r="AK40" s="5"/>
       <c r="AL40" s="5"/>
-      <c r="AM40" s="5"/>
+      <c r="AM40" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AN40" s="5" t="s">
         <v>71</v>
       </c>
@@ -4349,48 +4593,55 @@
       <c r="AS40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AT40" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AT40" s="5"/>
       <c r="AU40" s="5"/>
       <c r="AV40" s="5"/>
       <c r="AW40" s="5"/>
-      <c r="AX40" s="5"/>
+      <c r="AX40" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AY40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AZ40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BA40" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AZ40" s="5"/>
+      <c r="BA40" s="5"/>
       <c r="BB40" s="5"/>
       <c r="BC40" s="5"/>
-      <c r="BD40" s="5"/>
+      <c r="BD40" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BE40" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BF40" s="5"/>
+      <c r="BF40" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG40" s="5"/>
       <c r="BH40" s="5"/>
       <c r="BI40" s="5"/>
-      <c r="BJ40" s="5"/>
-      <c r="BK40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM40" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BJ40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BK40" s="5"/>
+      <c r="BL40" s="5"/>
+      <c r="BM40" s="5"/>
       <c r="BN40" s="5"/>
-      <c r="BO40" s="5" t="s">
+      <c r="BO40" s="5"/>
+      <c r="BP40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS40" s="5"/>
+      <c r="BT40" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -4460,8 +4711,13 @@
       <c r="BM41" s="6"/>
       <c r="BN41" s="6"/>
       <c r="BO41" s="6"/>
+      <c r="BP41" s="6"/>
+      <c r="BQ41" s="6"/>
+      <c r="BR41" s="6"/>
+      <c r="BS41" s="6"/>
+      <c r="BT41" s="6"/>
     </row>
-    <row r="42" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>55</v>
       </c>
@@ -4508,33 +4764,31 @@
       <c r="AF42" s="5"/>
       <c r="AG42" s="5"/>
       <c r="AH42" s="5"/>
-      <c r="AI42" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AI42" s="5"/>
       <c r="AJ42" s="5"/>
       <c r="AK42" s="5"/>
       <c r="AL42" s="5"/>
       <c r="AM42" s="5"/>
-      <c r="AN42" s="5"/>
+      <c r="AN42" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AO42" s="5"/>
       <c r="AP42" s="5"/>
       <c r="AQ42" s="5"/>
       <c r="AR42" s="5"/>
-      <c r="AS42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT42" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AS42" s="5"/>
+      <c r="AT42" s="5"/>
       <c r="AU42" s="5"/>
       <c r="AV42" s="5"/>
       <c r="AW42" s="5"/>
-      <c r="AX42" s="5"/>
-      <c r="AY42" s="5"/>
+      <c r="AX42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY42" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ42" s="5"/>
-      <c r="BA42" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA42" s="5"/>
       <c r="BB42" s="5"/>
       <c r="BC42" s="5"/>
       <c r="BD42" s="5"/>
@@ -4546,17 +4800,24 @@
       <c r="BH42" s="5"/>
       <c r="BI42" s="5"/>
       <c r="BJ42" s="5"/>
-      <c r="BK42" s="5"/>
-      <c r="BL42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM42" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL42" s="5"/>
+      <c r="BM42" s="5"/>
       <c r="BN42" s="5"/>
       <c r="BO42" s="5"/>
+      <c r="BP42" s="5"/>
+      <c r="BQ42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS42" s="5"/>
+      <c r="BT42" s="5"/>
     </row>
-    <row r="43" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>56</v>
       </c>
@@ -4600,28 +4861,28 @@
       <c r="AE43" s="5"/>
       <c r="AF43" s="5"/>
       <c r="AG43" s="5"/>
-      <c r="AH43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI43" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH43" s="5"/>
+      <c r="AI43" s="5"/>
       <c r="AJ43" s="5"/>
       <c r="AK43" s="5"/>
       <c r="AL43" s="5"/>
-      <c r="AM43" s="5"/>
-      <c r="AN43" s="5"/>
+      <c r="AM43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN43" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AO43" s="5"/>
       <c r="AP43" s="5"/>
       <c r="AQ43" s="5"/>
-      <c r="AR43" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AR43" s="5"/>
       <c r="AS43" s="5"/>
       <c r="AT43" s="5"/>
       <c r="AU43" s="5"/>
       <c r="AV43" s="5"/>
-      <c r="AW43" s="5"/>
+      <c r="AW43" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AX43" s="5"/>
       <c r="AY43" s="5"/>
       <c r="AZ43" s="5"/>
@@ -4633,23 +4894,28 @@
       <c r="BF43" s="5"/>
       <c r="BG43" s="5"/>
       <c r="BH43" s="5"/>
-      <c r="BI43" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI43" s="5"/>
       <c r="BJ43" s="5"/>
-      <c r="BK43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM43" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN43" s="5"/>
+      <c r="BK43" s="5"/>
+      <c r="BL43" s="5"/>
+      <c r="BM43" s="5"/>
+      <c r="BN43" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BO43" s="5"/>
+      <c r="BP43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS43" s="5"/>
+      <c r="BT43" s="5"/>
     </row>
-    <row r="44" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>57</v>
       </c>
@@ -4719,8 +4985,13 @@
       <c r="BM44" s="6"/>
       <c r="BN44" s="6"/>
       <c r="BO44" s="6"/>
+      <c r="BP44" s="6"/>
+      <c r="BQ44" s="6"/>
+      <c r="BR44" s="6"/>
+      <c r="BS44" s="6"/>
+      <c r="BT44" s="6"/>
     </row>
-    <row r="45" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>58</v>
       </c>
@@ -4772,72 +5043,79 @@
       </c>
       <c r="AD45" s="5"/>
       <c r="AE45" s="5"/>
-      <c r="AF45" s="5"/>
+      <c r="AF45" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AG45" s="5"/>
-      <c r="AH45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI45" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH45" s="5"/>
+      <c r="AI45" s="5"/>
       <c r="AJ45" s="5"/>
       <c r="AK45" s="5"/>
-      <c r="AL45" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AL45" s="5"/>
       <c r="AM45" s="5" t="s">
         <v>71</v>
       </c>
       <c r="AN45" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AP45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ45" s="5"/>
-      <c r="AR45" s="5"/>
-      <c r="AS45" s="5"/>
-      <c r="AT45" s="5"/>
-      <c r="AU45" s="5"/>
+      <c r="AO45" s="5"/>
+      <c r="AP45" s="5"/>
+      <c r="AQ45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AU45" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AV45" s="5"/>
       <c r="AW45" s="5"/>
       <c r="AX45" s="5"/>
       <c r="AY45" s="5"/>
       <c r="AZ45" s="5"/>
       <c r="BA45" s="5"/>
-      <c r="BB45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BC45" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BB45" s="5"/>
+      <c r="BC45" s="5"/>
       <c r="BD45" s="5"/>
       <c r="BE45" s="5"/>
       <c r="BF45" s="5"/>
-      <c r="BG45" s="5"/>
-      <c r="BH45" s="5"/>
-      <c r="BI45" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BG45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BI45" s="5"/>
       <c r="BJ45" s="5"/>
-      <c r="BK45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BL45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM45" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BN45" s="5"/>
-      <c r="BO45" s="5" t="s">
+      <c r="BK45" s="5"/>
+      <c r="BL45" s="5"/>
+      <c r="BM45" s="5"/>
+      <c r="BN45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BO45" s="5"/>
+      <c r="BP45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS45" s="5"/>
+      <c r="BT45" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>59</v>
       </c>
@@ -4879,30 +5157,34 @@
       <c r="AC46" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AD46" s="5"/>
+      <c r="AD46" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AE46" s="5"/>
       <c r="AF46" s="5"/>
       <c r="AG46" s="5"/>
-      <c r="AH46" s="5"/>
-      <c r="AI46" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH46" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI46" s="5"/>
       <c r="AJ46" s="5"/>
       <c r="AK46" s="5"/>
       <c r="AL46" s="5"/>
       <c r="AM46" s="5"/>
-      <c r="AN46" s="5"/>
+      <c r="AN46" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AO46" s="5"/>
       <c r="AP46" s="5"/>
       <c r="AQ46" s="5"/>
-      <c r="AR46" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AR46" s="5"/>
       <c r="AS46" s="5"/>
       <c r="AT46" s="5"/>
       <c r="AU46" s="5"/>
       <c r="AV46" s="5"/>
-      <c r="AW46" s="5"/>
+      <c r="AW46" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AX46" s="5"/>
       <c r="AY46" s="5"/>
       <c r="AZ46" s="5"/>
@@ -4921,8 +5203,13 @@
       <c r="BM46" s="5"/>
       <c r="BN46" s="5"/>
       <c r="BO46" s="5"/>
+      <c r="BP46" s="5"/>
+      <c r="BQ46" s="5"/>
+      <c r="BR46" s="5"/>
+      <c r="BS46" s="5"/>
+      <c r="BT46" s="5"/>
     </row>
-    <row r="47" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60</v>
       </c>
@@ -4958,9 +5245,7 @@
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
       <c r="AC47" s="5"/>
-      <c r="AD47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD47" s="5"/>
       <c r="AE47" s="5"/>
       <c r="AF47" s="5"/>
       <c r="AG47" s="5"/>
@@ -4968,24 +5253,26 @@
       <c r="AI47" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AJ47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AJ47" s="5"/>
       <c r="AK47" s="5"/>
       <c r="AL47" s="5"/>
       <c r="AM47" s="5"/>
-      <c r="AN47" s="5"/>
-      <c r="AO47" s="5"/>
+      <c r="AN47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO47" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AP47" s="5"/>
       <c r="AQ47" s="5"/>
-      <c r="AR47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AR47" s="5"/>
       <c r="AS47" s="5"/>
       <c r="AT47" s="5"/>
       <c r="AU47" s="5"/>
       <c r="AV47" s="5"/>
-      <c r="AW47" s="5"/>
+      <c r="AW47" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AX47" s="5"/>
       <c r="AY47" s="5"/>
       <c r="AZ47" s="5"/>
@@ -4993,29 +5280,34 @@
       <c r="BB47" s="5"/>
       <c r="BC47" s="5"/>
       <c r="BD47" s="5"/>
-      <c r="BE47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BE47" s="5"/>
       <c r="BF47" s="5"/>
-      <c r="BG47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BG47" s="5"/>
       <c r="BH47" s="5"/>
       <c r="BI47" s="5"/>
-      <c r="BJ47" s="5"/>
-      <c r="BK47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BJ47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BK47" s="5"/>
       <c r="BL47" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BM47" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BM47" s="5"/>
       <c r="BN47" s="5"/>
       <c r="BO47" s="5"/>
+      <c r="BP47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BQ47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR47" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS47" s="5"/>
+      <c r="BT47" s="5"/>
     </row>
-    <row r="48" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>61</v>
       </c>
@@ -5059,12 +5351,8 @@
       <c r="AE48" s="5"/>
       <c r="AF48" s="5"/>
       <c r="AG48" s="5"/>
-      <c r="AH48" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI48" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
       <c r="AJ48" s="5"/>
       <c r="AK48" s="5"/>
       <c r="AL48" s="5"/>
@@ -5074,12 +5362,12 @@
       <c r="AN48" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO48" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO48" s="5"/>
       <c r="AP48" s="5"/>
       <c r="AQ48" s="5"/>
-      <c r="AR48" s="5"/>
+      <c r="AR48" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AS48" s="5" t="s">
         <v>71</v>
       </c>
@@ -5089,32 +5377,41 @@
       <c r="AU48" s="5"/>
       <c r="AV48" s="5"/>
       <c r="AW48" s="5"/>
-      <c r="AX48" s="5"/>
-      <c r="AY48" s="5"/>
+      <c r="AX48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY48" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ48" s="5"/>
       <c r="BA48" s="5"/>
       <c r="BB48" s="5"/>
       <c r="BC48" s="5"/>
       <c r="BD48" s="5"/>
       <c r="BE48" s="5"/>
-      <c r="BF48" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BF48" s="5"/>
       <c r="BG48" s="5"/>
       <c r="BH48" s="5"/>
       <c r="BI48" s="5"/>
       <c r="BJ48" s="5"/>
-      <c r="BK48" s="5"/>
-      <c r="BL48" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL48" s="5"/>
       <c r="BM48" s="5"/>
-      <c r="BN48" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BN48" s="5"/>
       <c r="BO48" s="5"/>
+      <c r="BP48" s="5"/>
+      <c r="BQ48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR48" s="5"/>
+      <c r="BS48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT48" s="5"/>
     </row>
-    <row r="49" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>62</v>
       </c>
@@ -5162,22 +5459,18 @@
       <c r="AC49" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AD49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AD49" s="5"/>
       <c r="AE49" s="5"/>
-      <c r="AF49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AF49" s="5"/>
       <c r="AG49" s="5"/>
-      <c r="AH49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AH49" s="5"/>
       <c r="AI49" s="5" t="s">
         <v>71</v>
       </c>
       <c r="AJ49" s="5"/>
-      <c r="AK49" s="5"/>
+      <c r="AK49" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AL49" s="5"/>
       <c r="AM49" s="5" t="s">
         <v>71</v>
@@ -5185,12 +5478,12 @@
       <c r="AN49" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AO49" s="5"/>
       <c r="AP49" s="5"/>
       <c r="AQ49" s="5"/>
-      <c r="AR49" s="5"/>
+      <c r="AR49" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AS49" s="5" t="s">
         <v>71</v>
       </c>
@@ -5198,12 +5491,14 @@
         <v>71</v>
       </c>
       <c r="AU49" s="5"/>
-      <c r="AV49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AV49" s="5"/>
       <c r="AW49" s="5"/>
-      <c r="AX49" s="5"/>
-      <c r="AY49" s="5"/>
+      <c r="AX49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY49" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ49" s="5"/>
       <c r="BA49" s="5" t="s">
         <v>71</v>
@@ -5219,19 +5514,26 @@
       <c r="BH49" s="5"/>
       <c r="BI49" s="5"/>
       <c r="BJ49" s="5"/>
-      <c r="BK49" s="5"/>
-      <c r="BL49" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="BM49" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BK49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BL49" s="5"/>
+      <c r="BM49" s="5"/>
       <c r="BN49" s="5"/>
-      <c r="BO49" s="5" t="s">
+      <c r="BO49" s="5"/>
+      <c r="BP49" s="5"/>
+      <c r="BQ49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS49" s="5"/>
+      <c r="BT49" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>63</v>
       </c>
@@ -5274,18 +5576,14 @@
       <c r="AB50" s="5"/>
       <c r="AC50" s="5"/>
       <c r="AD50" s="5"/>
-      <c r="AE50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AE50" s="5"/>
       <c r="AF50" s="5"/>
-      <c r="AG50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AG50" s="5"/>
+      <c r="AH50" s="5"/>
       <c r="AI50" s="5"/>
-      <c r="AJ50" s="5"/>
+      <c r="AJ50" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AK50" s="5"/>
       <c r="AL50" s="5" t="s">
         <v>71</v>
@@ -5293,16 +5591,18 @@
       <c r="AM50" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AN50" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="AO50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="AN50" s="5"/>
+      <c r="AO50" s="5"/>
       <c r="AP50" s="5"/>
-      <c r="AQ50" s="5"/>
-      <c r="AR50" s="5"/>
-      <c r="AS50" s="5"/>
+      <c r="AQ50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS50" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AT50" s="5" t="s">
         <v>71</v>
       </c>
@@ -5310,44 +5610,52 @@
       <c r="AV50" s="5"/>
       <c r="AW50" s="5"/>
       <c r="AX50" s="5"/>
-      <c r="AY50" s="5"/>
+      <c r="AY50" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="AZ50" s="5"/>
-      <c r="BA50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BA50" s="5"/>
       <c r="BB50" s="5"/>
       <c r="BC50" s="5"/>
       <c r="BD50" s="5"/>
       <c r="BE50" s="5"/>
-      <c r="BF50" s="5"/>
+      <c r="BF50" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="BG50" s="5"/>
       <c r="BH50" s="5"/>
-      <c r="BI50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BI50" s="5"/>
       <c r="BJ50" s="5"/>
       <c r="BK50" s="5"/>
-      <c r="BL50" s="5" t="s">
-        <v>71</v>
-      </c>
+      <c r="BL50" s="5"/>
       <c r="BM50" s="5"/>
       <c r="BN50" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BO50" s="5" t="s">
+      <c r="BO50" s="5"/>
+      <c r="BP50" s="5"/>
+      <c r="BQ50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BR50" s="5"/>
+      <c r="BS50" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="BT50" s="5" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="BN1:BO1"/>
-    <mergeCell ref="AX1:BM1"/>
+  <mergeCells count="9">
+    <mergeCell ref="BS1:BT1"/>
+    <mergeCell ref="BC1:BR1"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="M1:Y1"/>
     <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AK1"/>
-    <mergeCell ref="AL1:AP1"/>
-    <mergeCell ref="AQ1:AW1"/>
+    <mergeCell ref="AI1:AP1"/>
+    <mergeCell ref="AQ1:AU1"/>
+    <mergeCell ref="AV1:BB1"/>
+    <mergeCell ref="AD1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>